<commit_message>
Final commit before print.
</commit_message>
<xml_diff>
--- a/plots/plot-runtime.xlsx
+++ b/plots/plot-runtime.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2780" windowWidth="28720" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="mean_runtime" localSheetId="0">Sheet1!$A$1:$C$14</definedName>
+    <definedName name="mean_runtime" localSheetId="1">Sheet1!$A$1:$C$14</definedName>
+    <definedName name="mean_runtime_1" localSheetId="0">Sheet2!$A$1:$C$7</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -40,16 +42,28 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="mean_runtime1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/bjohn/Desktop/datasets/svddd/02-rabbit/eval/mean_runtime.csv" comma="1" semicolon="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>algorithm</t>
   </si>
   <si>
-    <t>runtime</t>
+    <t>Cambridge</t>
+  </si>
+  <si>
+    <t>SVDDD</t>
   </si>
 </sst>
 </file>
@@ -131,7 +145,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>runtime</c:v>
+                  <c:v>Cambridge</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -147,6 +161,216 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0212071778140294"/>
+                  <c:y val="-0.00214132762312634"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00652528548123983"/>
+                  <c:y val="0.0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00489396411092985"/>
+                  <c:y val="0.00214132762312626"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.98144259300124E-17"/>
+                  <c:y val="-0.0107066381156318"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0293637846655791"/>
+                  <c:y val="-0.0599571734475375"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0146818923327896"/>
+                  <c:y val="-0.0192719486081371"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.00652528548123974"/>
+                  <c:y val="-0.00214132762312634"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00489396411092997"/>
+                  <c:y val="0.00214132762312634"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0032626427406199"/>
+                  <c:y val="-0.0107066381156317"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0130505709624797"/>
+                  <c:y val="-0.00214132762312638"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:numFmt formatCode="0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
@@ -253,6 +477,202 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVDDD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0163132137030995"/>
+                  <c:y val="0.00214132762312634"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0244698205546493"/>
+                  <c:y val="0.00642398286937901"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0277324632952692"/>
+                  <c:y val="0.00214132762312634"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0407830342577488"/>
+                  <c:y val="0.00856531049250535"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1650" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4402.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>465.230769231</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.21153846</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20141.2115385</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>420834.519231</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>617997.865385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
@@ -264,11 +684,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2141815744"/>
-        <c:axId val="-2141810032"/>
+        <c:axId val="2127349152"/>
+        <c:axId val="2127355328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2141815744"/>
+        <c:axId val="2127349152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -367,7 +787,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141810032"/>
+        <c:crossAx val="2127355328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -375,11 +795,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141810032"/>
+        <c:axId val="2127355328"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
-          <c:max val="150000.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1.0E6"/>
+          <c:min val="10.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -483,7 +904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141815744"/>
+        <c:crossAx val="2127349152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -495,6 +916,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1650" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1079,16 +1532,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1111,6 +1564,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mean_runtime_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mean_runtime" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -1377,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,6 +1851,81 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>465.23076923100001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1000.21153846</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>20141.2115385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>420834.51923099998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>617997.86538500001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>